<commit_message>
Modif midi Jeudi 04/07
Mise a l'echelle metrique sur 900 minutes + différenciation évolution métrique entre top 5 et top 15
</commit_message>
<xml_diff>
--- a/Tableau métriques/moyenne/2021_2022/Skill Corner/metrique_physical.xlsx
+++ b/Tableau métriques/moyenne/2021_2022/Skill Corner/metrique_physical.xlsx
@@ -577,82 +577,82 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40385.79411764706</v>
+        <v>38245.03311329238</v>
       </c>
       <c r="C2" t="n">
-        <v>1849.11</v>
+        <v>1757.557135943058</v>
       </c>
       <c r="D2" t="n">
-        <v>6547.794117647059</v>
+        <v>6200.304207411717</v>
       </c>
       <c r="E2" t="n">
-        <v>2512.882352941177</v>
+        <v>2381.49433727492</v>
       </c>
       <c r="F2" t="n">
-        <v>233.7352941176471</v>
+        <v>221.5532468662895</v>
       </c>
       <c r="G2" t="n">
-        <v>890.1176470588235</v>
+        <v>847.4837575814532</v>
       </c>
       <c r="H2" t="n">
-        <v>43.05882352941177</v>
+        <v>40.89049071784314</v>
       </c>
       <c r="I2" t="n">
-        <v>3403</v>
+        <v>3228.978094856374</v>
       </c>
       <c r="J2" t="n">
-        <v>276.7941176470588</v>
+        <v>262.4437375841327</v>
       </c>
       <c r="K2" t="n">
-        <v>406.2647058823529</v>
+        <v>384.5313542794729</v>
       </c>
       <c r="L2" t="n">
-        <v>26.55882352941176</v>
+        <v>25.17144328777763</v>
       </c>
       <c r="M2" t="n">
-        <v>292.7941176470588</v>
+        <v>276.9310007360748</v>
       </c>
       <c r="N2" t="n">
-        <v>41.94117647058823</v>
+        <v>39.70680705549299</v>
       </c>
       <c r="O2" t="n">
-        <v>32962.38235294117</v>
+        <v>31440.17263207441</v>
       </c>
       <c r="P2" t="n">
-        <v>1991.679117647059</v>
+        <v>1891.126053113459</v>
       </c>
       <c r="Q2" t="n">
-        <v>6501.411764705882</v>
+        <v>6189.874009047865</v>
       </c>
       <c r="R2" t="n">
-        <v>2662.235294117647</v>
+        <v>2532.094338317329</v>
       </c>
       <c r="S2" t="n">
-        <v>233.6764705882353</v>
+        <v>222.136886035803</v>
       </c>
       <c r="T2" t="n">
-        <v>653.3529411764706</v>
+        <v>621.4769208533244</v>
       </c>
       <c r="U2" t="n">
-        <v>33.35294117647059</v>
+        <v>31.67411357577021</v>
       </c>
       <c r="V2" t="n">
-        <v>3315.588235294118</v>
+        <v>3153.571259170653</v>
       </c>
       <c r="W2" t="n">
-        <v>267.0294117647059</v>
+        <v>253.8109996115732</v>
       </c>
       <c r="X2" t="n">
-        <v>360.2941176470588</v>
+        <v>343.6188554092861</v>
       </c>
       <c r="Y2" t="n">
-        <v>20.29411764705882</v>
+        <v>19.35495179734423</v>
       </c>
       <c r="Z2" t="n">
-        <v>258.4411764705882</v>
+        <v>246.6065971555531</v>
       </c>
       <c r="AA2" t="n">
-        <v>45.79411764705883</v>
+        <v>43.64389993789622</v>
       </c>
     </row>
     <row r="3">
@@ -662,82 +662,82 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>34507.02777777778</v>
+        <v>32499.04413726227</v>
       </c>
       <c r="C3" t="n">
-        <v>1896.481666666667</v>
+        <v>1786.609670827545</v>
       </c>
       <c r="D3" t="n">
-        <v>5713.138888888889</v>
+        <v>5378.734706132076</v>
       </c>
       <c r="E3" t="n">
-        <v>2132.555555555556</v>
+        <v>2007.90645452699</v>
       </c>
       <c r="F3" t="n">
-        <v>207.5833333333333</v>
+        <v>195.3979334832982</v>
       </c>
       <c r="G3" t="n">
-        <v>656.2222222222222</v>
+        <v>617.2524073440741</v>
       </c>
       <c r="H3" t="n">
-        <v>35.47222222222222</v>
+        <v>33.34520400626526</v>
       </c>
       <c r="I3" t="n">
-        <v>2788.777777777778</v>
+        <v>2625.158861871064</v>
       </c>
       <c r="J3" t="n">
-        <v>243.0555555555555</v>
+        <v>228.7431374895635</v>
       </c>
       <c r="K3" t="n">
-        <v>357.5555555555555</v>
+        <v>336.8281547835174</v>
       </c>
       <c r="L3" t="n">
-        <v>22.52777777777778</v>
+        <v>21.20098980071841</v>
       </c>
       <c r="M3" t="n">
-        <v>248.8611111111111</v>
+        <v>234.4034127069872</v>
       </c>
       <c r="N3" t="n">
-        <v>39.72222222222222</v>
+        <v>37.37377923268704</v>
       </c>
       <c r="O3" t="n">
-        <v>38497.86111111111</v>
+        <v>36289.31985932789</v>
       </c>
       <c r="P3" t="n">
-        <v>2017.574722222222</v>
+        <v>1900.827443428021</v>
       </c>
       <c r="Q3" t="n">
-        <v>7738.611111111111</v>
+        <v>7294.948835296573</v>
       </c>
       <c r="R3" t="n">
-        <v>2706.444444444444</v>
+        <v>2551.357721439193</v>
       </c>
       <c r="S3" t="n">
-        <v>248.7222222222222</v>
+        <v>234.3660304445436</v>
       </c>
       <c r="T3" t="n">
-        <v>602.2222222222222</v>
+        <v>566.7822713398243</v>
       </c>
       <c r="U3" t="n">
-        <v>33.44444444444444</v>
+        <v>31.4896106465157</v>
       </c>
       <c r="V3" t="n">
-        <v>3308.666666666667</v>
+        <v>3118.139992779018</v>
       </c>
       <c r="W3" t="n">
-        <v>282.1666666666667</v>
+        <v>265.8556410910593</v>
       </c>
       <c r="X3" t="n">
-        <v>406.1111111111111</v>
+        <v>382.8566004433583</v>
       </c>
       <c r="Y3" t="n">
-        <v>20.75</v>
+        <v>19.54214375698277</v>
       </c>
       <c r="Z3" t="n">
-        <v>298.3611111111111</v>
+        <v>281.3605260728197</v>
       </c>
       <c r="AA3" t="n">
-        <v>50.66666666666666</v>
+        <v>47.78193904311267</v>
       </c>
     </row>
     <row r="4">
@@ -747,82 +747,82 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>41912.60526315789</v>
+        <v>39835.65461768988</v>
       </c>
       <c r="C4" t="n">
-        <v>1727.025263157895</v>
+        <v>1642.562416926959</v>
       </c>
       <c r="D4" t="n">
-        <v>6197.184210526316</v>
+        <v>5888.771798129625</v>
       </c>
       <c r="E4" t="n">
-        <v>2330.078947368421</v>
+        <v>2214.43062076898</v>
       </c>
       <c r="F4" t="n">
-        <v>217.2368421052632</v>
+        <v>206.5063738952491</v>
       </c>
       <c r="G4" t="n">
-        <v>685</v>
+        <v>651.4409919283753</v>
       </c>
       <c r="H4" t="n">
-        <v>36.76315789473684</v>
+        <v>34.96197005383755</v>
       </c>
       <c r="I4" t="n">
-        <v>3015.078947368421</v>
+        <v>2865.871612697355</v>
       </c>
       <c r="J4" t="n">
-        <v>254</v>
+        <v>241.4683439490866</v>
       </c>
       <c r="K4" t="n">
-        <v>404.8421052631579</v>
+        <v>384.7696365088916</v>
       </c>
       <c r="L4" t="n">
-        <v>21.78947368421053</v>
+        <v>20.71681271646442</v>
       </c>
       <c r="M4" t="n">
-        <v>304</v>
+        <v>288.9744933766121</v>
       </c>
       <c r="N4" t="n">
-        <v>41.28947368421053</v>
+        <v>39.26688892702936</v>
       </c>
       <c r="O4" t="n">
-        <v>34712.5</v>
+        <v>33059.42705334981</v>
       </c>
       <c r="P4" t="n">
-        <v>1798.187631578948</v>
+        <v>1710.777219034276</v>
       </c>
       <c r="Q4" t="n">
-        <v>6148.973684210527</v>
+        <v>5854.851126469145</v>
       </c>
       <c r="R4" t="n">
-        <v>2448.5</v>
+        <v>2330.013959716519</v>
       </c>
       <c r="S4" t="n">
-        <v>224.4473684210526</v>
+        <v>213.6248492600263</v>
       </c>
       <c r="T4" t="n">
-        <v>652.078947368421</v>
+        <v>619.7484351617462</v>
       </c>
       <c r="U4" t="n">
-        <v>32</v>
+        <v>30.44134379420773</v>
       </c>
       <c r="V4" t="n">
-        <v>3100.578947368421</v>
+        <v>2949.762394878265</v>
       </c>
       <c r="W4" t="n">
-        <v>256.4473684210527</v>
+        <v>244.0661930542341</v>
       </c>
       <c r="X4" t="n">
-        <v>384.4473684210527</v>
+        <v>366.0246009398963</v>
       </c>
       <c r="Y4" t="n">
-        <v>18.31578947368421</v>
+        <v>17.43523994079843</v>
       </c>
       <c r="Z4" t="n">
-        <v>282.1842105263158</v>
+        <v>268.7016179673131</v>
       </c>
       <c r="AA4" t="n">
-        <v>44.8421052631579</v>
+        <v>42.72054323117423</v>
       </c>
     </row>
     <row r="5">
@@ -832,82 +832,82 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38335.78378378379</v>
+        <v>36329.3198039069</v>
       </c>
       <c r="C5" t="n">
-        <v>1898.26027027027</v>
+        <v>1796.3453528688</v>
       </c>
       <c r="D5" t="n">
-        <v>5786.027027027027</v>
+        <v>5485.629574808951</v>
       </c>
       <c r="E5" t="n">
-        <v>2377.081081081081</v>
+        <v>2253.566197583306</v>
       </c>
       <c r="F5" t="n">
-        <v>225.9459459459459</v>
+        <v>214.0807679957353</v>
       </c>
       <c r="G5" t="n">
-        <v>877.027027027027</v>
+        <v>831.1872437403199</v>
       </c>
       <c r="H5" t="n">
-        <v>44.24324324324324</v>
+        <v>41.92023953273372</v>
       </c>
       <c r="I5" t="n">
-        <v>3254.108108108108</v>
+        <v>3084.753441323626</v>
       </c>
       <c r="J5" t="n">
-        <v>270.1891891891892</v>
+        <v>256.001007528469</v>
       </c>
       <c r="K5" t="n">
-        <v>382.0810810810811</v>
+        <v>361.8716943300348</v>
       </c>
       <c r="L5" t="n">
-        <v>24.2972972972973</v>
+        <v>22.9985057976689</v>
       </c>
       <c r="M5" t="n">
-        <v>275.0810810810811</v>
+        <v>260.5669865292919</v>
       </c>
       <c r="N5" t="n">
-        <v>41.91891891891892</v>
+        <v>39.72274921270161</v>
       </c>
       <c r="O5" t="n">
-        <v>37869.81081081081</v>
+        <v>35826.4890328753</v>
       </c>
       <c r="P5" t="n">
-        <v>1979.268378378378</v>
+        <v>1873.92649046366</v>
       </c>
       <c r="Q5" t="n">
-        <v>6698.27027027027</v>
+        <v>6339.066088984951</v>
       </c>
       <c r="R5" t="n">
-        <v>2537.837837837838</v>
+        <v>2402.213546170371</v>
       </c>
       <c r="S5" t="n">
-        <v>244.2432432432433</v>
+        <v>231.0500634971331</v>
       </c>
       <c r="T5" t="n">
-        <v>717.4864864864865</v>
+        <v>679.3546493931528</v>
       </c>
       <c r="U5" t="n">
-        <v>36.21621621621622</v>
+        <v>34.26146077844262</v>
       </c>
       <c r="V5" t="n">
-        <v>3255.324324324324</v>
+        <v>3081.568195563524</v>
       </c>
       <c r="W5" t="n">
-        <v>280.4594594594595</v>
+        <v>265.3115242755757</v>
       </c>
       <c r="X5" t="n">
-        <v>428.0540540540541</v>
+        <v>404.7662379128714</v>
       </c>
       <c r="Y5" t="n">
-        <v>23.05405405405405</v>
+        <v>21.82375188926511</v>
       </c>
       <c r="Z5" t="n">
-        <v>307.972972972973</v>
+        <v>291.1439333807644</v>
       </c>
       <c r="AA5" t="n">
-        <v>55.4054054054054</v>
+        <v>52.40385255022856</v>
       </c>
     </row>
     <row r="6">
@@ -917,82 +917,82 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40759.02702702703</v>
+        <v>38364.30976201847</v>
       </c>
       <c r="C6" t="n">
-        <v>1927.291351351351</v>
+        <v>1813.472520353595</v>
       </c>
       <c r="D6" t="n">
-        <v>6848.837837837837</v>
+        <v>6443.928726638457</v>
       </c>
       <c r="E6" t="n">
-        <v>2502.054054054054</v>
+        <v>2354.562312141525</v>
       </c>
       <c r="F6" t="n">
-        <v>237.5405405405405</v>
+        <v>223.5256608571924</v>
       </c>
       <c r="G6" t="n">
-        <v>893.8648648648649</v>
+        <v>841.4474052927986</v>
       </c>
       <c r="H6" t="n">
-        <v>44.86486486486486</v>
+        <v>42.20616749958173</v>
       </c>
       <c r="I6" t="n">
-        <v>3395.918918918919</v>
+        <v>3196.009717434323</v>
       </c>
       <c r="J6" t="n">
-        <v>282.4054054054054</v>
+        <v>265.7318283567741</v>
       </c>
       <c r="K6" t="n">
-        <v>411.3243243243243</v>
+        <v>387.1249594865291</v>
       </c>
       <c r="L6" t="n">
-        <v>24.89189189189189</v>
+        <v>23.39365086153757</v>
       </c>
       <c r="M6" t="n">
-        <v>293.6216216216216</v>
+        <v>276.3745637222472</v>
       </c>
       <c r="N6" t="n">
-        <v>44.24324324324324</v>
+        <v>41.63703451013856</v>
       </c>
       <c r="O6" t="n">
-        <v>34321.59459459459</v>
+        <v>32315.64799448937</v>
       </c>
       <c r="P6" t="n">
-        <v>2014.263243243243</v>
+        <v>1895.49159348734</v>
       </c>
       <c r="Q6" t="n">
-        <v>6725.351351351352</v>
+        <v>6329.355380213569</v>
       </c>
       <c r="R6" t="n">
-        <v>2680.243243243243</v>
+        <v>2522.849394956393</v>
       </c>
       <c r="S6" t="n">
-        <v>247.0540540540541</v>
+        <v>232.5703907408471</v>
       </c>
       <c r="T6" t="n">
-        <v>726.1351351351351</v>
+        <v>683.3895994405326</v>
       </c>
       <c r="U6" t="n">
-        <v>36.54054054054054</v>
+        <v>34.39571636840808</v>
       </c>
       <c r="V6" t="n">
-        <v>3406.378378378378</v>
+        <v>3206.238994396926</v>
       </c>
       <c r="W6" t="n">
-        <v>283.5945945945946</v>
+        <v>266.9661071092552</v>
       </c>
       <c r="X6" t="n">
-        <v>388.6756756756757</v>
+        <v>365.9224841371235</v>
       </c>
       <c r="Y6" t="n">
-        <v>20.64864864864865</v>
+        <v>19.42781126609105</v>
       </c>
       <c r="Z6" t="n">
-        <v>273.7027027027027</v>
+        <v>257.7601949884595</v>
       </c>
       <c r="AA6" t="n">
-        <v>50.43243243243244</v>
+        <v>47.46906644811116</v>
       </c>
     </row>
     <row r="7">
@@ -1002,82 +1002,82 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38206.55555555555</v>
+        <v>35727.34822351123</v>
       </c>
       <c r="C7" t="n">
-        <v>1951.866111111111</v>
+        <v>1824.941744244175</v>
       </c>
       <c r="D7" t="n">
-        <v>6181.666666666667</v>
+        <v>5778.054733501265</v>
       </c>
       <c r="E7" t="n">
-        <v>2539.166666666667</v>
+        <v>2374.034468055822</v>
       </c>
       <c r="F7" t="n">
-        <v>239.9722222222222</v>
+        <v>224.3303883474233</v>
       </c>
       <c r="G7" t="n">
-        <v>922.8611111111111</v>
+        <v>862.4096956328447</v>
       </c>
       <c r="H7" t="n">
-        <v>47.25</v>
+        <v>44.17597803273693</v>
       </c>
       <c r="I7" t="n">
-        <v>3462.027777777778</v>
+        <v>3236.444163688667</v>
       </c>
       <c r="J7" t="n">
-        <v>287.2222222222222</v>
+        <v>268.5063663801603</v>
       </c>
       <c r="K7" t="n">
-        <v>399.9444444444445</v>
+        <v>373.9988628839857</v>
       </c>
       <c r="L7" t="n">
-        <v>24</v>
+        <v>22.42705974676062</v>
       </c>
       <c r="M7" t="n">
-        <v>284.8333333333333</v>
+        <v>266.3084704183372</v>
       </c>
       <c r="N7" t="n">
-        <v>42.63888888888889</v>
+        <v>39.84229381419119</v>
       </c>
       <c r="O7" t="n">
-        <v>38089.55555555555</v>
+        <v>35631.23939376771</v>
       </c>
       <c r="P7" t="n">
-        <v>2021.3325</v>
+        <v>1889.975864980121</v>
       </c>
       <c r="Q7" t="n">
-        <v>6992.361111111111</v>
+        <v>6538.871685802329</v>
       </c>
       <c r="R7" t="n">
-        <v>2730.722222222222</v>
+        <v>2553.280571057361</v>
       </c>
       <c r="S7" t="n">
-        <v>261.9444444444445</v>
+        <v>244.9416110812896</v>
       </c>
       <c r="T7" t="n">
-        <v>733</v>
+        <v>685.0519844463673</v>
       </c>
       <c r="U7" t="n">
-        <v>39.86111111111111</v>
+        <v>37.24662424277886</v>
       </c>
       <c r="V7" t="n">
-        <v>3463.722222222222</v>
+        <v>3238.332555503728</v>
       </c>
       <c r="W7" t="n">
-        <v>301.8055555555555</v>
+        <v>282.1882353240684</v>
       </c>
       <c r="X7" t="n">
-        <v>432.0277777777778</v>
+        <v>404.2059888197002</v>
       </c>
       <c r="Y7" t="n">
-        <v>22.02777777777778</v>
+        <v>20.576745637376</v>
       </c>
       <c r="Z7" t="n">
-        <v>310.8055555555555</v>
+        <v>290.8971981268087</v>
       </c>
       <c r="AA7" t="n">
-        <v>52.66666666666666</v>
+        <v>49.26548383392851</v>
       </c>
     </row>
     <row r="8">
@@ -1087,82 +1087,82 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>37318.57894736842</v>
+        <v>34951.32028616372</v>
       </c>
       <c r="C8" t="n">
-        <v>1869.25947368421</v>
+        <v>1751.151805984811</v>
       </c>
       <c r="D8" t="n">
-        <v>5915.684210526316</v>
+        <v>5539.375957080137</v>
       </c>
       <c r="E8" t="n">
-        <v>2363.78947368421</v>
+        <v>2214.672902506505</v>
       </c>
       <c r="F8" t="n">
-        <v>225.7105263157895</v>
+        <v>211.3902208503606</v>
       </c>
       <c r="G8" t="n">
-        <v>897.3684210526316</v>
+        <v>840.4830441363794</v>
       </c>
       <c r="H8" t="n">
-        <v>45.10526315789474</v>
+        <v>42.23366861559504</v>
       </c>
       <c r="I8" t="n">
-        <v>3261.157894736842</v>
+        <v>3055.155946642884</v>
       </c>
       <c r="J8" t="n">
-        <v>270.8157894736842</v>
+        <v>253.6238894659556</v>
       </c>
       <c r="K8" t="n">
-        <v>388.6842105263158</v>
+        <v>363.8326167412018</v>
       </c>
       <c r="L8" t="n">
-        <v>23.10526315789474</v>
+        <v>21.65071469694586</v>
       </c>
       <c r="M8" t="n">
-        <v>273.1315789473684</v>
+        <v>255.69757874504</v>
       </c>
       <c r="N8" t="n">
-        <v>40.5</v>
+        <v>37.9413581141843</v>
       </c>
       <c r="O8" t="n">
-        <v>38447.44736842105</v>
+        <v>36022.98809504891</v>
       </c>
       <c r="P8" t="n">
-        <v>1890.902105263158</v>
+        <v>1771.447233404109</v>
       </c>
       <c r="Q8" t="n">
-        <v>6898.315789473684</v>
+        <v>6460.413959497083</v>
       </c>
       <c r="R8" t="n">
-        <v>2665.78947368421</v>
+        <v>2495.709445324508</v>
       </c>
       <c r="S8" t="n">
-        <v>254.2105263157895</v>
+        <v>238.0490047412358</v>
       </c>
       <c r="T8" t="n">
-        <v>703.4736842105264</v>
+        <v>658.3429792237313</v>
       </c>
       <c r="U8" t="n">
-        <v>37.6578947368421</v>
+        <v>35.26213437837964</v>
       </c>
       <c r="V8" t="n">
-        <v>3369.263157894737</v>
+        <v>3154.052424548239</v>
       </c>
       <c r="W8" t="n">
-        <v>291.8684210526316</v>
+        <v>273.3111391196155</v>
       </c>
       <c r="X8" t="n">
-        <v>441.3157894736842</v>
+        <v>413.4399324186161</v>
       </c>
       <c r="Y8" t="n">
-        <v>21.65789473684211</v>
+        <v>20.2577579778538</v>
       </c>
       <c r="Z8" t="n">
-        <v>320.4473684210527</v>
+        <v>300.2766371495229</v>
       </c>
       <c r="AA8" t="n">
-        <v>54.57894736842105</v>
+        <v>51.06827590680861</v>
       </c>
     </row>
     <row r="9">
@@ -1172,82 +1172,82 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>33689.41666666666</v>
+        <v>31712.65601471566</v>
       </c>
       <c r="C9" t="n">
-        <v>1806.570833333333</v>
+        <v>1697.513342961181</v>
       </c>
       <c r="D9" t="n">
-        <v>5023.333333333333</v>
+        <v>4728.006377961241</v>
       </c>
       <c r="E9" t="n">
-        <v>2074.541666666667</v>
+        <v>1952.333528717393</v>
       </c>
       <c r="F9" t="n">
-        <v>204.75</v>
+        <v>192.5132950778745</v>
       </c>
       <c r="G9" t="n">
-        <v>749.0833333333334</v>
+        <v>704.3459205458515</v>
       </c>
       <c r="H9" t="n">
-        <v>39.16666666666666</v>
+        <v>36.80827451024174</v>
       </c>
       <c r="I9" t="n">
-        <v>2823.625</v>
+        <v>2656.679449263244</v>
       </c>
       <c r="J9" t="n">
-        <v>243.9166666666667</v>
+        <v>229.3215695881162</v>
       </c>
       <c r="K9" t="n">
-        <v>351.625</v>
+        <v>331.0493211637479</v>
       </c>
       <c r="L9" t="n">
-        <v>20</v>
+        <v>18.82247802464963</v>
       </c>
       <c r="M9" t="n">
-        <v>242.7083333333333</v>
+        <v>228.5377516086306</v>
       </c>
       <c r="N9" t="n">
-        <v>41.33333333333334</v>
+        <v>38.90880828022765</v>
       </c>
       <c r="O9" t="n">
-        <v>41080.875</v>
+        <v>38629.15028659082</v>
       </c>
       <c r="P9" t="n">
-        <v>2028.800416666667</v>
+        <v>1906.544449689495</v>
       </c>
       <c r="Q9" t="n">
-        <v>7503.875</v>
+        <v>7057.538681514773</v>
       </c>
       <c r="R9" t="n">
-        <v>2791.041666666667</v>
+        <v>2625.852751651979</v>
       </c>
       <c r="S9" t="n">
-        <v>266.25</v>
+        <v>250.3188464636979</v>
       </c>
       <c r="T9" t="n">
-        <v>744.875</v>
+        <v>700.7098024968385</v>
       </c>
       <c r="U9" t="n">
-        <v>40.16666666666666</v>
+        <v>37.74508253750755</v>
       </c>
       <c r="V9" t="n">
-        <v>3535.916666666667</v>
+        <v>3326.562554148817</v>
       </c>
       <c r="W9" t="n">
-        <v>306.4166666666667</v>
+        <v>288.0639290012055</v>
       </c>
       <c r="X9" t="n">
-        <v>461.125</v>
+        <v>433.0815423552864</v>
       </c>
       <c r="Y9" t="n">
-        <v>21.33333333333333</v>
+        <v>19.99893606800926</v>
       </c>
       <c r="Z9" t="n">
-        <v>333.375</v>
+        <v>313.2265431193254</v>
       </c>
       <c r="AA9" t="n">
-        <v>58.91666666666666</v>
+        <v>55.35588011076818</v>
       </c>
     </row>
     <row r="10">
@@ -1257,82 +1257,82 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>36746.08333333334</v>
+        <v>34599.30578078904</v>
       </c>
       <c r="C10" t="n">
-        <v>1925.231944444445</v>
+        <v>1813.768055238299</v>
       </c>
       <c r="D10" t="n">
-        <v>5988.222222222223</v>
+        <v>5636.938385052741</v>
       </c>
       <c r="E10" t="n">
-        <v>2301.25</v>
+        <v>2165.221969408223</v>
       </c>
       <c r="F10" t="n">
-        <v>210.5833333333333</v>
+        <v>198.1199025707598</v>
       </c>
       <c r="G10" t="n">
-        <v>706.7222222222222</v>
+        <v>664.0143623256224</v>
       </c>
       <c r="H10" t="n">
-        <v>37.25</v>
+        <v>35.03201147873428</v>
       </c>
       <c r="I10" t="n">
-        <v>3007.972222222222</v>
+        <v>2829.236331733845</v>
       </c>
       <c r="J10" t="n">
-        <v>247.8333333333333</v>
+        <v>233.1519140494941</v>
       </c>
       <c r="K10" t="n">
-        <v>369.6388888888889</v>
+        <v>348.0469324585746</v>
       </c>
       <c r="L10" t="n">
-        <v>19.16666666666667</v>
+        <v>18.02493926423912</v>
       </c>
       <c r="M10" t="n">
-        <v>258.25</v>
+        <v>243.1907355472126</v>
       </c>
       <c r="N10" t="n">
-        <v>39.08333333333334</v>
+        <v>36.78198422600281</v>
       </c>
       <c r="O10" t="n">
-        <v>40379.80555555555</v>
+        <v>38013.70916507281</v>
       </c>
       <c r="P10" t="n">
-        <v>2052.549722222222</v>
+        <v>1934.21398782214</v>
       </c>
       <c r="Q10" t="n">
-        <v>7546.361111111111</v>
+        <v>7104.278146511607</v>
       </c>
       <c r="R10" t="n">
-        <v>2686.222222222222</v>
+        <v>2530.029499378603</v>
       </c>
       <c r="S10" t="n">
-        <v>242.1388888888889</v>
+        <v>228.0049846634972</v>
       </c>
       <c r="T10" t="n">
-        <v>644.1666666666666</v>
+        <v>607.239011985018</v>
       </c>
       <c r="U10" t="n">
-        <v>32.38888888888889</v>
+        <v>30.51344935987909</v>
       </c>
       <c r="V10" t="n">
-        <v>3330.388888888889</v>
+        <v>3137.26851136362</v>
       </c>
       <c r="W10" t="n">
-        <v>274.5277777777778</v>
+        <v>258.5184340233763</v>
       </c>
       <c r="X10" t="n">
-        <v>421.75</v>
+        <v>397.0339840138156</v>
       </c>
       <c r="Y10" t="n">
-        <v>20.30555555555556</v>
+        <v>19.09787495587503</v>
       </c>
       <c r="Z10" t="n">
-        <v>312.4722222222222</v>
+        <v>294.1851427522167</v>
       </c>
       <c r="AA10" t="n">
-        <v>49.55555555555556</v>
+        <v>46.66148726448649</v>
       </c>
     </row>
     <row r="11">
@@ -1342,82 +1342,82 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35518.89189189189</v>
+        <v>33556.87371432573</v>
       </c>
       <c r="C11" t="n">
-        <v>1918.657027027027</v>
+        <v>1814.323322454931</v>
       </c>
       <c r="D11" t="n">
-        <v>5570.891891891892</v>
+        <v>5260.150160628757</v>
       </c>
       <c r="E11" t="n">
-        <v>2326.567567567567</v>
+        <v>2196.798965504275</v>
       </c>
       <c r="F11" t="n">
-        <v>221.9189189189189</v>
+        <v>209.5475429531017</v>
       </c>
       <c r="G11" t="n">
-        <v>815.1081081081081</v>
+        <v>769.2388941444563</v>
       </c>
       <c r="H11" t="n">
-        <v>40.86486486486486</v>
+        <v>38.5938364196981</v>
       </c>
       <c r="I11" t="n">
-        <v>3141.675675675676</v>
+        <v>2966.037859648732</v>
       </c>
       <c r="J11" t="n">
-        <v>262.7837837837838</v>
+        <v>248.1413793727997</v>
       </c>
       <c r="K11" t="n">
-        <v>358.6216216216216</v>
+        <v>338.6410023512584</v>
       </c>
       <c r="L11" t="n">
-        <v>21.67567567567568</v>
+        <v>20.44505142322577</v>
       </c>
       <c r="M11" t="n">
-        <v>250.9189189189189</v>
+        <v>236.9468140317591</v>
       </c>
       <c r="N11" t="n">
-        <v>39.72972972972973</v>
+        <v>37.53058492236872</v>
       </c>
       <c r="O11" t="n">
-        <v>39901.54054054054</v>
+        <v>37795.27953249563</v>
       </c>
       <c r="P11" t="n">
-        <v>2010.063243243243</v>
+        <v>1902.70474997408</v>
       </c>
       <c r="Q11" t="n">
-        <v>7082.972972972973</v>
+        <v>6709.321416079494</v>
       </c>
       <c r="R11" t="n">
-        <v>2451.783783783784</v>
+        <v>2320.804939557562</v>
       </c>
       <c r="S11" t="n">
-        <v>234.4324324324324</v>
+        <v>221.8202145568863</v>
       </c>
       <c r="T11" t="n">
-        <v>677.3243243243244</v>
+        <v>640.4599988154947</v>
       </c>
       <c r="U11" t="n">
-        <v>33.35135135135135</v>
+        <v>31.51960780515648</v>
       </c>
       <c r="V11" t="n">
-        <v>3129.108108108108</v>
+        <v>2961.264938373056</v>
       </c>
       <c r="W11" t="n">
-        <v>267.7837837837838</v>
+        <v>253.3398223620428</v>
       </c>
       <c r="X11" t="n">
-        <v>420.6486486486486</v>
+        <v>398.2331604895535</v>
       </c>
       <c r="Y11" t="n">
-        <v>21.27027027027027</v>
+        <v>20.11182949080873</v>
       </c>
       <c r="Z11" t="n">
-        <v>317.7297297297297</v>
+        <v>300.9267137088569</v>
       </c>
       <c r="AA11" t="n">
-        <v>50.78378378378378</v>
+        <v>48.10667988009593</v>
       </c>
     </row>
     <row r="12">
@@ -1427,82 +1427,82 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>34042.34285714286</v>
+        <v>31924.77795037885</v>
       </c>
       <c r="C12" t="n">
-        <v>1820.498285714286</v>
+        <v>1709.226529569799</v>
       </c>
       <c r="D12" t="n">
-        <v>5280.742857142857</v>
+        <v>4951.300566856832</v>
       </c>
       <c r="E12" t="n">
-        <v>2119.971428571429</v>
+        <v>1989.14131314416</v>
       </c>
       <c r="F12" t="n">
-        <v>200.9714285714286</v>
+        <v>188.511910952724</v>
       </c>
       <c r="G12" t="n">
-        <v>710.7428571428571</v>
+        <v>667.0945804989935</v>
       </c>
       <c r="H12" t="n">
-        <v>36.62857142857143</v>
+        <v>34.36742642369819</v>
       </c>
       <c r="I12" t="n">
-        <v>2830.714285714286</v>
+        <v>2656.235893643154</v>
       </c>
       <c r="J12" t="n">
-        <v>237.6</v>
+        <v>222.8793373764222</v>
       </c>
       <c r="K12" t="n">
-        <v>344.6857142857143</v>
+        <v>323.1572713646102</v>
       </c>
       <c r="L12" t="n">
-        <v>20.68571428571429</v>
+        <v>19.40959774174423</v>
       </c>
       <c r="M12" t="n">
-        <v>237.0571428571428</v>
+        <v>222.1603472937751</v>
       </c>
       <c r="N12" t="n">
-        <v>36.11428571428571</v>
+        <v>33.83238760043948</v>
       </c>
       <c r="O12" t="n">
-        <v>39516.94285714286</v>
+        <v>37177.20980042957</v>
       </c>
       <c r="P12" t="n">
-        <v>2004.805428571429</v>
+        <v>1882.029628096796</v>
       </c>
       <c r="Q12" t="n">
-        <v>7443.571428571428</v>
+        <v>6997.97720980198</v>
       </c>
       <c r="R12" t="n">
-        <v>3141.771428571429</v>
+        <v>2951.406684730563</v>
       </c>
       <c r="S12" t="n">
-        <v>289.7428571428571</v>
+        <v>272.2086915090495</v>
       </c>
       <c r="T12" t="n">
-        <v>893.8571428571429</v>
+        <v>839.1136476804604</v>
       </c>
       <c r="U12" t="n">
-        <v>47.22857142857143</v>
+        <v>44.37879488398616</v>
       </c>
       <c r="V12" t="n">
-        <v>4035.628571428571</v>
+        <v>3790.520332411023</v>
       </c>
       <c r="W12" t="n">
-        <v>336.9714285714286</v>
+        <v>316.5874863930357</v>
       </c>
       <c r="X12" t="n">
-        <v>430.5428571428571</v>
+        <v>404.8806935345627</v>
       </c>
       <c r="Y12" t="n">
-        <v>23.14285714285714</v>
+        <v>21.74811024745186</v>
       </c>
       <c r="Z12" t="n">
-        <v>312.3428571428572</v>
+        <v>293.8804295773204</v>
       </c>
       <c r="AA12" t="n">
-        <v>54.14285714285715</v>
+        <v>50.92385965164715</v>
       </c>
     </row>
     <row r="13">
@@ -1512,82 +1512,82 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>35389.58333333334</v>
+        <v>33400.81349215898</v>
       </c>
       <c r="C13" t="n">
-        <v>1858.859166666666</v>
+        <v>1753.497097978196</v>
       </c>
       <c r="D13" t="n">
-        <v>5820.583333333333</v>
+        <v>5492.744281768415</v>
       </c>
       <c r="E13" t="n">
-        <v>2206.25</v>
+        <v>2081.617532743563</v>
       </c>
       <c r="F13" t="n">
-        <v>202.6111111111111</v>
+        <v>191.1969619314859</v>
       </c>
       <c r="G13" t="n">
-        <v>645.6388888888889</v>
+        <v>609.0852414515706</v>
       </c>
       <c r="H13" t="n">
-        <v>34.22222222222222</v>
+        <v>32.26976470417866</v>
       </c>
       <c r="I13" t="n">
-        <v>2851.888888888889</v>
+        <v>2690.702774195134</v>
       </c>
       <c r="J13" t="n">
-        <v>236.8333333333333</v>
+        <v>223.4667266356646</v>
       </c>
       <c r="K13" t="n">
-        <v>355.6666666666667</v>
+        <v>335.7716657760849</v>
       </c>
       <c r="L13" t="n">
-        <v>19.27777777777778</v>
+        <v>18.17784094726269</v>
       </c>
       <c r="M13" t="n">
-        <v>252.8888888888889</v>
+        <v>238.7297038298212</v>
       </c>
       <c r="N13" t="n">
-        <v>39.91666666666666</v>
+        <v>37.66836162969642</v>
       </c>
       <c r="O13" t="n">
-        <v>39108.58333333334</v>
+        <v>36883.66617384075</v>
       </c>
       <c r="P13" t="n">
-        <v>1951.356666666667</v>
+        <v>1840.583584579148</v>
       </c>
       <c r="Q13" t="n">
-        <v>7528.583333333333</v>
+        <v>7100.825748611669</v>
       </c>
       <c r="R13" t="n">
-        <v>2719.166666666667</v>
+        <v>2564.479362394357</v>
       </c>
       <c r="S13" t="n">
-        <v>246.6666666666667</v>
+        <v>232.6371150823617</v>
       </c>
       <c r="T13" t="n">
-        <v>638.6666666666666</v>
+        <v>601.7674645570363</v>
       </c>
       <c r="U13" t="n">
-        <v>33.30555555555556</v>
+        <v>31.38321765866515</v>
       </c>
       <c r="V13" t="n">
-        <v>3357.833333333333</v>
+        <v>3166.246826951393</v>
       </c>
       <c r="W13" t="n">
-        <v>279.9722222222222</v>
+        <v>264.0203327410269</v>
       </c>
       <c r="X13" t="n">
-        <v>447.1388888888889</v>
+        <v>421.6225187593739</v>
       </c>
       <c r="Y13" t="n">
-        <v>20.11111111111111</v>
+        <v>18.9610097184604</v>
       </c>
       <c r="Z13" t="n">
-        <v>332</v>
+        <v>313.0607988831151</v>
       </c>
       <c r="AA13" t="n">
-        <v>52.08333333333334</v>
+        <v>49.10175908112218</v>
       </c>
     </row>
     <row r="14">
@@ -1597,82 +1597,82 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>34381.70967741936</v>
+        <v>32689.01741591886</v>
       </c>
       <c r="C14" t="n">
-        <v>1794.498709677419</v>
+        <v>1701.174526645647</v>
       </c>
       <c r="D14" t="n">
-        <v>5383</v>
+        <v>5112.88799434892</v>
       </c>
       <c r="E14" t="n">
-        <v>2069.903225806452</v>
+        <v>1964.282481062862</v>
       </c>
       <c r="F14" t="n">
-        <v>197.9354838709677</v>
+        <v>187.7923593051985</v>
       </c>
       <c r="G14" t="n">
-        <v>657.4516129032259</v>
+        <v>624.7304372284598</v>
       </c>
       <c r="H14" t="n">
-        <v>34.12903225806452</v>
+        <v>32.37312598259111</v>
       </c>
       <c r="I14" t="n">
-        <v>2727.354838709678</v>
+        <v>2589.012918291322</v>
       </c>
       <c r="J14" t="n">
-        <v>232.0645161290323</v>
+        <v>220.1654852877896</v>
       </c>
       <c r="K14" t="n">
-        <v>355</v>
+        <v>337.2911964459875</v>
       </c>
       <c r="L14" t="n">
-        <v>19.38709677419355</v>
+        <v>18.38693421152254</v>
       </c>
       <c r="M14" t="n">
-        <v>245.258064516129</v>
+        <v>233.117807080912</v>
       </c>
       <c r="N14" t="n">
-        <v>36</v>
+        <v>34.21036933884186</v>
       </c>
       <c r="O14" t="n">
-        <v>42921.1935483871</v>
+        <v>40668.16497309941</v>
       </c>
       <c r="P14" t="n">
-        <v>1954.573225806452</v>
+        <v>1853.31725983307</v>
       </c>
       <c r="Q14" t="n">
-        <v>8353.322580645161</v>
+        <v>7913.337624110826</v>
       </c>
       <c r="R14" t="n">
-        <v>3161.548387096774</v>
+        <v>2996.468541485473</v>
       </c>
       <c r="S14" t="n">
-        <v>298.0322580645162</v>
+        <v>282.3192247311213</v>
       </c>
       <c r="T14" t="n">
-        <v>870.1935483870968</v>
+        <v>825.5512108868013</v>
       </c>
       <c r="U14" t="n">
-        <v>46.38709677419355</v>
+        <v>43.97405884210976</v>
       </c>
       <c r="V14" t="n">
-        <v>4031.741935483871</v>
+        <v>3822.019752372274</v>
       </c>
       <c r="W14" t="n">
-        <v>344.4193548387097</v>
+        <v>326.2932835732311</v>
       </c>
       <c r="X14" t="n">
-        <v>467.516129032258</v>
+        <v>443.1763366070703</v>
       </c>
       <c r="Y14" t="n">
-        <v>22.32258064516129</v>
+        <v>21.16522445671716</v>
       </c>
       <c r="Z14" t="n">
-        <v>343.516129032258</v>
+        <v>325.5251420143118</v>
       </c>
       <c r="AA14" t="n">
-        <v>55.29032258064516</v>
+        <v>52.36861314931601</v>
       </c>
     </row>
     <row r="15">
@@ -1682,82 +1682,82 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>36523.81081081081</v>
+        <v>34622.12060813731</v>
       </c>
       <c r="C15" t="n">
-        <v>1896.951621621622</v>
+        <v>1798.640002538314</v>
       </c>
       <c r="D15" t="n">
-        <v>5499.243243243243</v>
+        <v>5211.75227434212</v>
       </c>
       <c r="E15" t="n">
-        <v>2171.945945945946</v>
+        <v>2058.586320347985</v>
       </c>
       <c r="F15" t="n">
-        <v>204</v>
+        <v>193.3570242230889</v>
       </c>
       <c r="G15" t="n">
-        <v>749.1081081081081</v>
+        <v>709.8461316887618</v>
       </c>
       <c r="H15" t="n">
-        <v>37.21621621621622</v>
+        <v>35.25963866816105</v>
       </c>
       <c r="I15" t="n">
-        <v>2921.054054054054</v>
+        <v>2768.432452036747</v>
       </c>
       <c r="J15" t="n">
-        <v>241.2162162162162</v>
+        <v>228.6166628912499</v>
       </c>
       <c r="K15" t="n">
-        <v>367.4864864864865</v>
+        <v>348.2456417825973</v>
       </c>
       <c r="L15" t="n">
-        <v>21.94594594594595</v>
+        <v>20.78726325078235</v>
       </c>
       <c r="M15" t="n">
-        <v>262.7837837837838</v>
+        <v>249.0724970614975</v>
       </c>
       <c r="N15" t="n">
-        <v>39.91891891891892</v>
+        <v>37.82702651580312</v>
       </c>
       <c r="O15" t="n">
-        <v>37846.45945945946</v>
+        <v>35956.11748919122</v>
       </c>
       <c r="P15" t="n">
-        <v>2017.786486486487</v>
+        <v>1914.32467951373</v>
       </c>
       <c r="Q15" t="n">
-        <v>6997.081081081081</v>
+        <v>6648.11881062922</v>
       </c>
       <c r="R15" t="n">
-        <v>2707.783783783784</v>
+        <v>2571.577495722455</v>
       </c>
       <c r="S15" t="n">
-        <v>254.2162162162162</v>
+        <v>241.3841052808941</v>
       </c>
       <c r="T15" t="n">
-        <v>729.7837837837837</v>
+        <v>692.7725020088776</v>
       </c>
       <c r="U15" t="n">
-        <v>38.5945945945946</v>
+        <v>36.62463872834574</v>
       </c>
       <c r="V15" t="n">
-        <v>3437.567567567567</v>
+        <v>3264.349997731333</v>
       </c>
       <c r="W15" t="n">
-        <v>292.8108108108108</v>
+        <v>278.0087440092399</v>
       </c>
       <c r="X15" t="n">
-        <v>423.8648648648648</v>
+        <v>402.5917815805749</v>
       </c>
       <c r="Y15" t="n">
-        <v>21.7027027027027</v>
+        <v>20.58818266223681</v>
       </c>
       <c r="Z15" t="n">
-        <v>310.6486486486486</v>
+        <v>295.1599233991067</v>
       </c>
       <c r="AA15" t="n">
-        <v>50.83783783783784</v>
+        <v>48.25928335638009</v>
       </c>
     </row>
     <row r="16">
@@ -1767,82 +1767,82 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>32669.34285714286</v>
+        <v>30834.49821083745</v>
       </c>
       <c r="C16" t="n">
-        <v>1931.034285714286</v>
+        <v>1824.955169983611</v>
       </c>
       <c r="D16" t="n">
-        <v>5094.828571428571</v>
+        <v>4808.138677226871</v>
       </c>
       <c r="E16" t="n">
-        <v>2082.428571428572</v>
+        <v>1966.247746387659</v>
       </c>
       <c r="F16" t="n">
-        <v>196.8571428571429</v>
+        <v>185.8928085102627</v>
       </c>
       <c r="G16" t="n">
-        <v>723.5428571428571</v>
+        <v>684.0892388843872</v>
       </c>
       <c r="H16" t="n">
-        <v>36.48571428571429</v>
+        <v>34.48313997859874</v>
       </c>
       <c r="I16" t="n">
-        <v>2805.971428571429</v>
+        <v>2650.336985272047</v>
       </c>
       <c r="J16" t="n">
-        <v>233.3428571428572</v>
+        <v>220.3759484888615</v>
       </c>
       <c r="K16" t="n">
-        <v>335.1142857142857</v>
+        <v>316.4500301182314</v>
       </c>
       <c r="L16" t="n">
-        <v>19.65714285714286</v>
+        <v>18.55154460157359</v>
       </c>
       <c r="M16" t="n">
-        <v>237.4857142857143</v>
+        <v>224.1898755806921</v>
       </c>
       <c r="N16" t="n">
-        <v>36.14285714285715</v>
+        <v>34.12680711643406</v>
       </c>
       <c r="O16" t="n">
-        <v>41618</v>
+        <v>39333.47810827673</v>
       </c>
       <c r="P16" t="n">
-        <v>2063.444571428571</v>
+        <v>1950.234577710387</v>
       </c>
       <c r="Q16" t="n">
-        <v>7702.057142857143</v>
+        <v>7275.18438381999</v>
       </c>
       <c r="R16" t="n">
-        <v>2815.485714285714</v>
+        <v>2661.962250527356</v>
       </c>
       <c r="S16" t="n">
-        <v>256.8</v>
+        <v>242.7975147658969</v>
       </c>
       <c r="T16" t="n">
-        <v>699.3428571428572</v>
+        <v>662.3447190965047</v>
       </c>
       <c r="U16" t="n">
-        <v>34.62857142857143</v>
+        <v>32.7655537530103</v>
       </c>
       <c r="V16" t="n">
-        <v>3514.828571428572</v>
+        <v>3324.306969623861</v>
       </c>
       <c r="W16" t="n">
-        <v>291.4285714285714</v>
+        <v>275.5630685189072</v>
       </c>
       <c r="X16" t="n">
-        <v>460.4285714285714</v>
+        <v>435.2114100255834</v>
       </c>
       <c r="Y16" t="n">
-        <v>20.31428571428571</v>
+        <v>19.19037990539216</v>
       </c>
       <c r="Z16" t="n">
-        <v>346.9714285714286</v>
+        <v>327.9275164545384</v>
       </c>
       <c r="AA16" t="n">
-        <v>54.22857142857143</v>
+        <v>51.24997588561863</v>
       </c>
     </row>
     <row r="17">
@@ -1852,82 +1852,82 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>33838.23684210526</v>
+        <v>32197.91631945951</v>
       </c>
       <c r="C17" t="n">
-        <v>1896.463421052632</v>
+        <v>1805.582730617899</v>
       </c>
       <c r="D17" t="n">
-        <v>5557.973684210527</v>
+        <v>5287.461061073574</v>
       </c>
       <c r="E17" t="n">
-        <v>2290.657894736842</v>
+        <v>2182.108513671355</v>
       </c>
       <c r="F17" t="n">
-        <v>210.421052631579</v>
+        <v>200.337664868818</v>
       </c>
       <c r="G17" t="n">
-        <v>767.9473684210526</v>
+        <v>733.223326592201</v>
       </c>
       <c r="H17" t="n">
-        <v>38.94736842105263</v>
+        <v>37.13326301539426</v>
       </c>
       <c r="I17" t="n">
-        <v>3058.605263157895</v>
+        <v>2915.331840263556</v>
       </c>
       <c r="J17" t="n">
-        <v>249.3684210526316</v>
+        <v>237.4709278842122</v>
       </c>
       <c r="K17" t="n">
-        <v>342.3684210526316</v>
+        <v>325.5494735320646</v>
       </c>
       <c r="L17" t="n">
-        <v>18.52631578947368</v>
+        <v>17.62620049982698</v>
       </c>
       <c r="M17" t="n">
-        <v>239.1842105263158</v>
+        <v>227.2553887637085</v>
       </c>
       <c r="N17" t="n">
-        <v>38.02631578947368</v>
+        <v>36.11733105354341</v>
       </c>
       <c r="O17" t="n">
-        <v>40117.36842105263</v>
+        <v>38227.21615555442</v>
       </c>
       <c r="P17" t="n">
-        <v>2003.093947368421</v>
+        <v>1907.749988971838</v>
       </c>
       <c r="Q17" t="n">
-        <v>7560.657894736843</v>
+        <v>7201.163201644224</v>
       </c>
       <c r="R17" t="n">
-        <v>2807.394736842105</v>
+        <v>2671.698051368409</v>
       </c>
       <c r="S17" t="n">
-        <v>257.7105263157895</v>
+        <v>245.2744887391809</v>
       </c>
       <c r="T17" t="n">
-        <v>740.1842105263158</v>
+        <v>703.5289181469866</v>
       </c>
       <c r="U17" t="n">
-        <v>38</v>
+        <v>36.12723154371011</v>
       </c>
       <c r="V17" t="n">
-        <v>3547.578947368421</v>
+        <v>3375.226969515396</v>
       </c>
       <c r="W17" t="n">
-        <v>295.7105263157895</v>
+        <v>281.4017202828911</v>
       </c>
       <c r="X17" t="n">
-        <v>431.5263157894737</v>
+        <v>411.1229662586708</v>
       </c>
       <c r="Y17" t="n">
-        <v>19.39473684210526</v>
+        <v>18.45047282502311</v>
       </c>
       <c r="Z17" t="n">
-        <v>323.8684210526316</v>
+        <v>308.5979099002224</v>
       </c>
       <c r="AA17" t="n">
-        <v>50.23684210526316</v>
+        <v>47.84697068360161</v>
       </c>
     </row>
     <row r="18">
@@ -1937,82 +1937,82 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>34514.86486486487</v>
+        <v>32464.62477656585</v>
       </c>
       <c r="C18" t="n">
-        <v>2039.48945945946</v>
+        <v>1917.084750358108</v>
       </c>
       <c r="D18" t="n">
-        <v>6083.621621621622</v>
+        <v>5720.668541323336</v>
       </c>
       <c r="E18" t="n">
-        <v>2443.567567567567</v>
+        <v>2298.195199375691</v>
       </c>
       <c r="F18" t="n">
-        <v>220.7297297297297</v>
+        <v>207.5244364210596</v>
       </c>
       <c r="G18" t="n">
-        <v>727.972972972973</v>
+        <v>685.2584542983894</v>
       </c>
       <c r="H18" t="n">
-        <v>39.18918918918919</v>
+        <v>36.89834281183595</v>
       </c>
       <c r="I18" t="n">
-        <v>3171.54054054054</v>
+        <v>2983.453653674081</v>
       </c>
       <c r="J18" t="n">
-        <v>259.9189189189189</v>
+        <v>244.4227792328955</v>
       </c>
       <c r="K18" t="n">
-        <v>348.9189189189189</v>
+        <v>328.1650305555928</v>
       </c>
       <c r="L18" t="n">
-        <v>20.35135135135135</v>
+        <v>19.13552302802644</v>
       </c>
       <c r="M18" t="n">
-        <v>246.7297297297297</v>
+        <v>231.9727766106595</v>
       </c>
       <c r="N18" t="n">
-        <v>38.32432432432432</v>
+        <v>36.04145555465609</v>
       </c>
       <c r="O18" t="n">
-        <v>42336.67567567567</v>
+        <v>39861.06727929034</v>
       </c>
       <c r="P18" t="n">
-        <v>2117.182702702702</v>
+        <v>1990.21486077696</v>
       </c>
       <c r="Q18" t="n">
-        <v>7855.027027027027</v>
+        <v>7394.432913796735</v>
       </c>
       <c r="R18" t="n">
-        <v>3002.675675675676</v>
+        <v>2824.042567216219</v>
       </c>
       <c r="S18" t="n">
-        <v>274.0540540540541</v>
+        <v>257.8007822823</v>
       </c>
       <c r="T18" t="n">
-        <v>823</v>
+        <v>772.2808620996474</v>
       </c>
       <c r="U18" t="n">
-        <v>41.24324324324324</v>
+        <v>38.75414424911429</v>
       </c>
       <c r="V18" t="n">
-        <v>3825.675675675676</v>
+        <v>3596.323429315867</v>
       </c>
       <c r="W18" t="n">
-        <v>315.2972972972973</v>
+        <v>296.5549265314143</v>
       </c>
       <c r="X18" t="n">
-        <v>461.2162162162162</v>
+        <v>434.0992711116339</v>
       </c>
       <c r="Y18" t="n">
-        <v>23.72972972972973</v>
+        <v>22.32968082193736</v>
       </c>
       <c r="Z18" t="n">
-        <v>342.2702702702703</v>
+        <v>322.3668549959459</v>
       </c>
       <c r="AA18" t="n">
-        <v>57.05405405405406</v>
+        <v>53.73533695125183</v>
       </c>
     </row>
     <row r="19">
@@ -2022,82 +2022,82 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>32054.20588235294</v>
+        <v>30119.38859742292</v>
       </c>
       <c r="C19" t="n">
-        <v>1849.456176470588</v>
+        <v>1736.66476249109</v>
       </c>
       <c r="D19" t="n">
-        <v>5146.264705882353</v>
+        <v>4836.715978468995</v>
       </c>
       <c r="E19" t="n">
-        <v>2047.411764705882</v>
+        <v>1923.973250434202</v>
       </c>
       <c r="F19" t="n">
-        <v>191.3529411764706</v>
+        <v>179.8137021520933</v>
       </c>
       <c r="G19" t="n">
-        <v>651.5882352941177</v>
+        <v>611.904366424434</v>
       </c>
       <c r="H19" t="n">
-        <v>33.35294117647059</v>
+        <v>31.33086458238964</v>
       </c>
       <c r="I19" t="n">
-        <v>2699</v>
+        <v>2535.877616858636</v>
       </c>
       <c r="J19" t="n">
-        <v>224.7058823529412</v>
+        <v>211.1445667344829</v>
       </c>
       <c r="K19" t="n">
-        <v>336.7941176470588</v>
+        <v>316.4643785870497</v>
       </c>
       <c r="L19" t="n">
-        <v>20.67647058823529</v>
+        <v>19.39716607790639</v>
       </c>
       <c r="M19" t="n">
-        <v>230.2941176470588</v>
+        <v>216.5225582828384</v>
       </c>
       <c r="N19" t="n">
-        <v>33.91176470588236</v>
+        <v>31.89491258960997</v>
       </c>
       <c r="O19" t="n">
-        <v>40608.64705882353</v>
+        <v>38094.13135671659</v>
       </c>
       <c r="P19" t="n">
-        <v>1972.682352941176</v>
+        <v>1851.720301729615</v>
       </c>
       <c r="Q19" t="n">
-        <v>7307.058823529412</v>
+        <v>6853.158811800633</v>
       </c>
       <c r="R19" t="n">
-        <v>2751.058823529412</v>
+        <v>2581.829539908847</v>
       </c>
       <c r="S19" t="n">
-        <v>268.7941176470588</v>
+        <v>252.1425839410952</v>
       </c>
       <c r="T19" t="n">
-        <v>754.7058823529412</v>
+        <v>707.9335520738163</v>
       </c>
       <c r="U19" t="n">
-        <v>40.35294117647059</v>
+        <v>37.84568357156233</v>
       </c>
       <c r="V19" t="n">
-        <v>3505.764705882353</v>
+        <v>3289.763091982663</v>
       </c>
       <c r="W19" t="n">
-        <v>309.1470588235294</v>
+        <v>289.9882675126575</v>
       </c>
       <c r="X19" t="n">
-        <v>466.6176470588235</v>
+        <v>437.8126496536024</v>
       </c>
       <c r="Y19" t="n">
-        <v>23.58823529411765</v>
+        <v>22.13134435005868</v>
       </c>
       <c r="Z19" t="n">
-        <v>343.0294117647059</v>
+        <v>321.762715523745</v>
       </c>
       <c r="AA19" t="n">
-        <v>56.05882352941177</v>
+        <v>52.6380912882653</v>
       </c>
     </row>
     <row r="20">
@@ -2107,82 +2107,82 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>32215.66666666667</v>
+        <v>30156.84747066248</v>
       </c>
       <c r="C20" t="n">
-        <v>1936.888611111111</v>
+        <v>1814.044874241087</v>
       </c>
       <c r="D20" t="n">
-        <v>5247.361111111111</v>
+        <v>4911.175893357597</v>
       </c>
       <c r="E20" t="n">
-        <v>2093.138888888889</v>
+        <v>1959.178689402509</v>
       </c>
       <c r="F20" t="n">
-        <v>196.4722222222222</v>
+        <v>183.8348164877708</v>
       </c>
       <c r="G20" t="n">
-        <v>700.8333333333334</v>
+        <v>655.7587942333535</v>
       </c>
       <c r="H20" t="n">
-        <v>35.83333333333334</v>
+        <v>33.52550380775735</v>
       </c>
       <c r="I20" t="n">
-        <v>2793.972222222222</v>
+        <v>2614.937483635863</v>
       </c>
       <c r="J20" t="n">
-        <v>232.3055555555555</v>
+        <v>217.3603202955282</v>
       </c>
       <c r="K20" t="n">
-        <v>333.6666666666667</v>
+        <v>312.2836216826745</v>
       </c>
       <c r="L20" t="n">
-        <v>21.16666666666667</v>
+        <v>19.81446849970185</v>
       </c>
       <c r="M20" t="n">
-        <v>232.5277777777778</v>
+        <v>217.6542408808185</v>
       </c>
       <c r="N20" t="n">
-        <v>38.27777777777778</v>
+        <v>35.81817550107806</v>
       </c>
       <c r="O20" t="n">
-        <v>40059.25</v>
+        <v>37572.19880266338</v>
       </c>
       <c r="P20" t="n">
-        <v>2079.126666666667</v>
+        <v>1947.71611415023</v>
       </c>
       <c r="Q20" t="n">
-        <v>7699.416666666667</v>
+        <v>7220.206106041735</v>
       </c>
       <c r="R20" t="n">
-        <v>2870.694444444444</v>
+        <v>2691.761931028316</v>
       </c>
       <c r="S20" t="n">
-        <v>264.9166666666667</v>
+        <v>248.4006198059043</v>
       </c>
       <c r="T20" t="n">
-        <v>738.4444444444445</v>
+        <v>692.3382162146625</v>
       </c>
       <c r="U20" t="n">
-        <v>39.91666666666666</v>
+        <v>37.41803846101172</v>
       </c>
       <c r="V20" t="n">
-        <v>3609.138888888889</v>
+        <v>3384.100147242978</v>
       </c>
       <c r="W20" t="n">
-        <v>304.8333333333333</v>
+        <v>285.818658266916</v>
       </c>
       <c r="X20" t="n">
-        <v>442.3333333333333</v>
+        <v>414.7442705052798</v>
       </c>
       <c r="Y20" t="n">
-        <v>23.27777777777778</v>
+        <v>21.82259785782909</v>
       </c>
       <c r="Z20" t="n">
-        <v>321.9722222222222</v>
+        <v>301.9781936940815</v>
       </c>
       <c r="AA20" t="n">
-        <v>54.27777777777778</v>
+        <v>50.90108159053389</v>
       </c>
     </row>
     <row r="21">
@@ -2192,82 +2192,82 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>36992.11111111111</v>
+        <v>35156.95476618902</v>
       </c>
       <c r="C21" t="n">
-        <v>1905.3975</v>
+        <v>1814.791029582654</v>
       </c>
       <c r="D21" t="n">
-        <v>6275.472222222223</v>
+        <v>5968.638919531206</v>
       </c>
       <c r="E21" t="n">
-        <v>2392.083333333333</v>
+        <v>2274.696901113578</v>
       </c>
       <c r="F21" t="n">
-        <v>220.2222222222222</v>
+        <v>209.3587300746551</v>
       </c>
       <c r="G21" t="n">
-        <v>825.25</v>
+        <v>783.5486663241466</v>
       </c>
       <c r="H21" t="n">
-        <v>41.55555555555556</v>
+        <v>39.46282914811896</v>
       </c>
       <c r="I21" t="n">
-        <v>3217.333333333333</v>
+        <v>3058.245567437725</v>
       </c>
       <c r="J21" t="n">
-        <v>261.7777777777778</v>
+        <v>248.8215592227741</v>
       </c>
       <c r="K21" t="n">
-        <v>380.2222222222222</v>
+        <v>361.2164668351104</v>
       </c>
       <c r="L21" t="n">
-        <v>22.36111111111111</v>
+        <v>21.22087414459916</v>
       </c>
       <c r="M21" t="n">
-        <v>266.2777777777778</v>
+        <v>252.8409996131148</v>
       </c>
       <c r="N21" t="n">
-        <v>42.22222222222222</v>
+        <v>40.0997764924509</v>
       </c>
       <c r="O21" t="n">
-        <v>37074.5</v>
+        <v>35375.18827407724</v>
       </c>
       <c r="P21" t="n">
-        <v>2031.496944444444</v>
+        <v>1936.834205860589</v>
       </c>
       <c r="Q21" t="n">
-        <v>7297.388888888889</v>
+        <v>6966.144843695444</v>
       </c>
       <c r="R21" t="n">
-        <v>2823.527777777778</v>
+        <v>2695.798690905988</v>
       </c>
       <c r="S21" t="n">
-        <v>250.4722222222222</v>
+        <v>239.065753471853</v>
       </c>
       <c r="T21" t="n">
-        <v>758.6111111111111</v>
+        <v>724.1259617438004</v>
       </c>
       <c r="U21" t="n">
-        <v>38.44444444444444</v>
+        <v>36.7165519629629</v>
       </c>
       <c r="V21" t="n">
-        <v>3582.138888888889</v>
+        <v>3419.924652649789</v>
       </c>
       <c r="W21" t="n">
-        <v>288.9166666666667</v>
+        <v>275.7823054348158</v>
       </c>
       <c r="X21" t="n">
-        <v>399.1944444444445</v>
+        <v>380.8147797481968</v>
       </c>
       <c r="Y21" t="n">
-        <v>21.38888888888889</v>
+        <v>20.33850763009366</v>
       </c>
       <c r="Z21" t="n">
-        <v>286.75</v>
+        <v>273.5815285978683</v>
       </c>
       <c r="AA21" t="n">
-        <v>52.22222222222222</v>
+        <v>49.8018655397398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>